<commit_message>
Updating T20 Standings table
</commit_message>
<xml_diff>
--- a/data/t20_standings.xlsx
+++ b/data/t20_standings.xlsx
@@ -53,6 +53,18 @@
     <t>Peshawar Zalmi</t>
   </si>
   <si>
+    <t>CodeCricketMaster</t>
+  </si>
+  <si>
+    <t>Sydney Sixers</t>
+  </si>
+  <si>
+    <t>GentleGamer</t>
+  </si>
+  <si>
+    <t>Multan Sultans</t>
+  </si>
+  <si>
     <t>Rahul</t>
   </si>
   <si>
@@ -65,12 +77,6 @@
     <t>Barbados Royals</t>
   </si>
   <si>
-    <t>GentleGamer</t>
-  </si>
-  <si>
-    <t>Multan Sultans</t>
-  </si>
-  <si>
     <t>Mike</t>
   </si>
   <si>
@@ -83,10 +89,16 @@
     <t>Chennai Super Kings</t>
   </si>
   <si>
-    <t>CodeCricketMaster</t>
-  </si>
-  <si>
-    <t>Sydney Sixers</t>
+    <t>Ved</t>
+  </si>
+  <si>
+    <t>Kolkata Knight Riders</t>
+  </si>
+  <si>
+    <t>Dosu</t>
+  </si>
+  <si>
+    <t>Guyana Amazon Warriors</t>
   </si>
   <si>
     <t>newGuy</t>
@@ -95,40 +107,46 @@
     <t>St Lucia Kings</t>
   </si>
   <si>
+    <t>sammat</t>
+  </si>
+  <si>
+    <t>Karachi Kings</t>
+  </si>
+  <si>
+    <t>Sricharan</t>
+  </si>
+  <si>
+    <t>Melbourne Stars</t>
+  </si>
+  <si>
     <t>Sachin</t>
   </si>
   <si>
     <t>Melbourne Renegades</t>
   </si>
   <si>
-    <t>sammat</t>
-  </si>
-  <si>
-    <t>Karachi Kings</t>
-  </si>
-  <si>
-    <t>Sricharan</t>
-  </si>
-  <si>
-    <t>Melbourne Stars</t>
-  </si>
-  <si>
-    <t>Ved</t>
-  </si>
-  <si>
-    <t>Kolkata Knight Riders</t>
-  </si>
-  <si>
     <t>Crabby</t>
   </si>
   <si>
     <t>Hobart Hurricanes</t>
   </si>
   <si>
-    <t>dosu</t>
-  </si>
-  <si>
-    <t>Guyana Amazon Warriors</t>
+    <t>AnkitGamer</t>
+  </si>
+  <si>
+    <t>Rajasthan Royals</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Delhi Capitals</t>
+  </si>
+  <si>
+    <t>GeniiExE</t>
+  </si>
+  <si>
+    <t>Adelaide Strikers</t>
   </si>
   <si>
     <t>ady_chak</t>
@@ -137,10 +155,16 @@
     <t>Mumbai Indians</t>
   </si>
   <si>
-    <t>Angel</t>
-  </si>
-  <si>
-    <t>Delhi Capitals</t>
+    <t>Prateesh</t>
+  </si>
+  <si>
+    <t>Perth Scorchers</t>
+  </si>
+  <si>
+    <t>Maverick</t>
+  </si>
+  <si>
+    <t>Brisbane Heat</t>
   </si>
   <si>
     <t>Ava</t>
@@ -149,34 +173,10 @@
     <t>Punjab Kings</t>
   </si>
   <si>
-    <t>GeniiExE</t>
-  </si>
-  <si>
-    <t>Adelaide Strikers</t>
-  </si>
-  <si>
-    <t>Prateesh</t>
-  </si>
-  <si>
-    <t>Perth Scorchers</t>
-  </si>
-  <si>
     <t>Bawandar</t>
   </si>
   <si>
     <t>Sydney Thunder</t>
-  </si>
-  <si>
-    <t>Maverick</t>
-  </si>
-  <si>
-    <t>Brisbane Heat</t>
-  </si>
-  <si>
-    <t>AnkitGamer</t>
-  </si>
-  <si>
-    <t>Rajasthan Royals</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,13 +199,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -675,155 +668,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1174,7 +1170,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1183,7 +1179,7 @@
     <col min="2" max="2" width="23.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="15.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="13.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="5.22222222222222" customWidth="1"/>
+    <col min="5" max="5" width="20.4444444444444" customWidth="1"/>
     <col min="6" max="6" width="6.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1215,16 +1211,16 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1235,16 +1231,16 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1255,16 +1251,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-1.7</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1335,13 +1331,13 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-4.25</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1351,59 +1347,59 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1411,19 +1407,19 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1431,19 +1427,19 @@
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1451,19 +1447,19 @@
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-1.82</v>
+      </c>
+      <c r="F14" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1471,179 +1467,179 @@
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-4.45</v>
+      </c>
+      <c r="F15" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-0.86</v>
+      </c>
+      <c r="F16" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4.9</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>-0.86</v>
+      </c>
+      <c r="F22" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-3.92</v>
+      </c>
+      <c r="F23" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding articles page. Updating t20 standings
</commit_message>
<xml_diff>
--- a/data/t20_standings.xlsx
+++ b/data/t20_standings.xlsx
@@ -47,30 +47,30 @@
     <t>Points</t>
   </si>
   <si>
+    <t>RunMachine</t>
+  </si>
+  <si>
+    <t>Barbados Royals</t>
+  </si>
+  <si>
     <t>QuantumQuirk</t>
   </si>
   <si>
     <t>Peshawar Zalmi</t>
   </si>
   <si>
+    <t>GentleGamer</t>
+  </si>
+  <si>
+    <t>Multan Sultans</t>
+  </si>
+  <si>
     <t>CodeCricketMaster</t>
   </si>
   <si>
     <t>Sydney Sixers</t>
   </si>
   <si>
-    <t>RunMachine</t>
-  </si>
-  <si>
-    <t>Barbados Royals</t>
-  </si>
-  <si>
-    <t>GentleGamer</t>
-  </si>
-  <si>
-    <t>Multan Sultans</t>
-  </si>
-  <si>
     <t>db1_db2</t>
   </si>
   <si>
@@ -89,30 +89,30 @@
     <t>Sunrisers Hyderabad</t>
   </si>
   <si>
+    <t>dosu</t>
+  </si>
+  <si>
+    <t>Guyana Amazon Warriors</t>
+  </si>
+  <si>
+    <t>Ved</t>
+  </si>
+  <si>
+    <t>Kolkata Knight Riders</t>
+  </si>
+  <si>
     <t>sammat</t>
   </si>
   <si>
     <t>Karachi Kings</t>
   </si>
   <si>
-    <t>Ved</t>
-  </si>
-  <si>
-    <t>Kolkata Knight Riders</t>
-  </si>
-  <si>
     <t>newGuy</t>
   </si>
   <si>
     <t>St Lucia Kings</t>
   </si>
   <si>
-    <t>dosu</t>
-  </si>
-  <si>
-    <t>Guyana Amazon Warriors</t>
-  </si>
-  <si>
     <t>Crabby</t>
   </si>
   <si>
@@ -131,46 +131,46 @@
     <t>Melbourne Renegades</t>
   </si>
   <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Delhi Capitals</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Punjab Kings</t>
+  </si>
+  <si>
+    <t>ady_chak</t>
+  </si>
+  <si>
+    <t>Mumbai Indians</t>
+  </si>
+  <si>
     <t>Maverick</t>
   </si>
   <si>
     <t>Brisbane Heat</t>
   </si>
   <si>
-    <t>Angel</t>
-  </si>
-  <si>
-    <t>Delhi Capitals</t>
+    <t>Prateesh</t>
+  </si>
+  <si>
+    <t>Perth Scorchers</t>
+  </si>
+  <si>
+    <t>GeniiExE</t>
+  </si>
+  <si>
+    <t>Adelaide Strikers</t>
   </si>
   <si>
     <t>AnkitGamer</t>
   </si>
   <si>
     <t>Rajasthan Royals</t>
-  </si>
-  <si>
-    <t>Ava</t>
-  </si>
-  <si>
-    <t>Punjab Kings</t>
-  </si>
-  <si>
-    <t>ady_chak</t>
-  </si>
-  <si>
-    <t>Mumbai Indians</t>
-  </si>
-  <si>
-    <t>Prateesh</t>
-  </si>
-  <si>
-    <t>Perth Scorchers</t>
-  </si>
-  <si>
-    <t>GeniiExE</t>
-  </si>
-  <si>
-    <t>Adelaide Strikers</t>
   </si>
   <si>
     <t>Bawandar</t>
@@ -1177,7 +1177,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1218,16 +1218,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.2</v>
+        <v>0.39</v>
       </c>
       <c r="F2" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1238,16 +1238,16 @@
         <v>9</v>
       </c>
       <c r="C3" s="2">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
-        <v>4</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.9</v>
+        <v>-0.04</v>
       </c>
       <c r="F3" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1258,16 +1258,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.53</v>
+        <v>-0.26</v>
       </c>
       <c r="F4" s="2">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1278,16 +1278,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
-        <v>3</v>
-      </c>
       <c r="E5" s="2">
-        <v>-0.32</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1298,16 +1298,16 @@
         <v>15</v>
       </c>
       <c r="C6" s="2">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
       <c r="E6" s="2">
-        <v>-0.76</v>
+        <v>0.32</v>
       </c>
       <c r="F6" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1318,16 +1318,16 @@
         <v>17</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>-0.21</v>
+        <v>0.74</v>
       </c>
       <c r="F7" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1338,16 +1338,16 @@
         <v>19</v>
       </c>
       <c r="C8" s="2">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-1.76</v>
+      </c>
+      <c r="F8" s="2">
         <v>6</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>-0.57</v>
-      </c>
-      <c r="F8" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1358,16 +1358,16 @@
         <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.81</v>
+        <v>0.22</v>
       </c>
       <c r="F9" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1378,16 +1378,16 @@
         <v>23</v>
       </c>
       <c r="C10" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>-0.23</v>
+        <v>0.45</v>
       </c>
       <c r="F10" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1398,16 +1398,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="2">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
         <v>7</v>
       </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
       <c r="E11" s="2">
-        <v>1.67</v>
+        <v>0.42</v>
       </c>
       <c r="F11" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1418,16 +1418,16 @@
         <v>27</v>
       </c>
       <c r="C12" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2">
-        <v>0.39</v>
+        <v>0.27</v>
       </c>
       <c r="F12" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1438,16 +1438,16 @@
         <v>29</v>
       </c>
       <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="D13" s="2">
-        <v>3</v>
-      </c>
       <c r="E13" s="2">
-        <v>0.78</v>
+        <v>-0.1</v>
       </c>
       <c r="F13" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1458,16 +1458,16 @@
         <v>31</v>
       </c>
       <c r="C14" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>-1.19</v>
+        <v>-0.44</v>
       </c>
       <c r="F14" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1478,16 +1478,16 @@
         <v>33</v>
       </c>
       <c r="C15" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2">
-        <v>-1.79</v>
+        <v>-0.86</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1498,16 +1498,16 @@
         <v>35</v>
       </c>
       <c r="C16" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2">
-        <v>1.08</v>
+        <v>0.32</v>
       </c>
       <c r="F16" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1518,16 +1518,16 @@
         <v>37</v>
       </c>
       <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2">
         <v>8</v>
       </c>
-      <c r="D17" s="2">
-        <v>6</v>
-      </c>
       <c r="E17" s="2">
-        <v>0.94</v>
+        <v>0.81</v>
       </c>
       <c r="F17" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1538,16 +1538,16 @@
         <v>39</v>
       </c>
       <c r="C18" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2">
-        <v>-0.94</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1558,16 +1558,16 @@
         <v>41</v>
       </c>
       <c r="C19" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2">
         <v>0.35</v>
       </c>
       <c r="F19" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1578,16 +1578,16 @@
         <v>43</v>
       </c>
       <c r="C20" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E20" s="2">
-        <v>-0.04</v>
+        <v>0.37</v>
       </c>
       <c r="F20" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1598,16 +1598,16 @@
         <v>45</v>
       </c>
       <c r="C21" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2">
-        <v>-0.1</v>
+        <v>0.13</v>
       </c>
       <c r="F21" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1618,16 +1618,16 @@
         <v>47</v>
       </c>
       <c r="C22" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2">
-        <v>-0.47</v>
+        <v>-0.98</v>
       </c>
       <c r="F22" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1638,16 +1638,16 @@
         <v>49</v>
       </c>
       <c r="C23" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D23" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" s="2">
-        <v>-1.99</v>
+        <v>-1.02</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>